<commit_message>
Se agregó la función de densidad en las librerías
</commit_message>
<xml_diff>
--- a/50datosdelanzamientosexitosos.xlsx
+++ b/50datosdelanzamientosexitosos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SERGIO ROMO\Documents\Semestre 2021-1\Temas Selectos de Programación\Lanzamientos Espaciales Exitosos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC1E21A-3C53-44D4-8B19-1AD4C03212F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2E74B6-3FC8-49FD-AADC-87E1BB8D2FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C12EC2E4-22FE-4489-88A3-7C800461580F}"/>
   </bookViews>
@@ -222,13 +222,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6448,7 +6448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4B0B39-51E5-4F5E-8BA1-E0453CD653D3}">
   <dimension ref="A1:BF88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
@@ -6475,11 +6475,11 @@
       <c r="B2" s="5">
         <v>112</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -6496,10 +6496,10 @@
       <c r="B4" s="5">
         <v>105</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <f>SUM(B2:B51)</f>
         <v>4577</v>
       </c>
@@ -6511,10 +6511,10 @@
       <c r="B5" s="2">
         <v>109</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <f>AVERAGE(B2:B51)</f>
         <v>91.54</v>
       </c>
@@ -6722,10 +6722,10 @@
       <c r="B6" s="5">
         <v>105</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <f>MIN(B2:B51)</f>
         <v>50</v>
       </c>
@@ -6737,10 +6737,10 @@
       <c r="B7" s="2">
         <v>124</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <f>MAX(B2:B51)</f>
         <v>127</v>
       </c>
@@ -6908,11 +6908,11 @@
       <c r="B27" s="2">
         <v>72</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
@@ -6921,10 +6921,10 @@
       <c r="B28" s="5">
         <v>69</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -6933,18 +6933,18 @@
       <c r="B29" s="2">
         <v>83</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9">
+      <c r="E29" s="7"/>
+      <c r="F29" s="7">
         <f>_xlfn.VAR.P(B2:B51)</f>
         <v>501.60840000000002</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="7">
         <f>$E$5+$F$31</f>
         <v>113.93661581578789</v>
       </c>
@@ -7152,18 +7152,18 @@
       <c r="B30" s="5">
         <v>75</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9">
+      <c r="E30" s="7"/>
+      <c r="F30" s="7">
         <f>_xlfn.VAR.S(B2:B51)</f>
         <v>511.84530612244862</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="7">
         <f>$E$5+($F$31*2)</f>
         <v>136.33323163157579</v>
       </c>
@@ -7371,18 +7371,18 @@
       <c r="B31" s="2">
         <v>73</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9">
+      <c r="E31" s="7"/>
+      <c r="F31" s="7">
         <f>_xlfn.STDEV.P(B2:B51)</f>
         <v>22.396615815787886</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="7">
         <f>$E$5+($F$31*3)</f>
         <v>158.72984744736368</v>
       </c>
@@ -7590,18 +7590,18 @@
       <c r="B32" s="5">
         <v>81</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9">
+      <c r="E32" s="7"/>
+      <c r="F32" s="7">
         <f>_xlfn.STDEV.S(B2:B51)</f>
         <v>22.623998455676411</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H32" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="7">
         <f>$E$5+($F$31*4)</f>
         <v>181.12646326315155</v>
       </c>
@@ -7817,10 +7817,10 @@
       <c r="B34" s="5">
         <v>60</v>
       </c>
-      <c r="H34" s="9" t="s">
+      <c r="H34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I34" s="9"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -7829,10 +7829,10 @@
       <c r="B35" s="2">
         <v>60</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="H35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I35" s="7">
         <f>$E$5-$F$31</f>
         <v>69.143384184212124</v>
       </c>
@@ -8040,10 +8040,10 @@
       <c r="B36" s="5">
         <v>50</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H36" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I36" s="9">
+      <c r="I36" s="7">
         <f>$E$5-($F$31*2)</f>
         <v>46.746768368424235</v>
       </c>
@@ -8251,10 +8251,10 @@
       <c r="B37" s="2">
         <v>52</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I37" s="9">
+      <c r="I37" s="7">
         <f>$E$5-($F$31*3)</f>
         <v>24.350152552636345</v>
       </c>
@@ -8465,10 +8465,10 @@
       <c r="D38" t="s">
         <v>10</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="H38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="7">
         <f>$E$5-($F$31*4)</f>
         <v>1.9535367368484629</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>63</v>
       </c>
       <c r="D39">
-        <f>(B2-$E$5)^2</f>
+        <f t="shared" ref="D39:D70" si="9">(B2-$E$5)^2</f>
         <v>418.61159999999973</v>
       </c>
     </row>
@@ -8689,7 +8689,7 @@
         <v>66</v>
       </c>
       <c r="D40">
-        <f>(B3-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>754.05159999999967</v>
       </c>
       <c r="E40" t="s">
@@ -8708,7 +8708,7 @@
         <v>73</v>
       </c>
       <c r="D41">
-        <f>(B4-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>181.17159999999984</v>
       </c>
       <c r="E41" t="s">
@@ -8727,7 +8727,7 @@
         <v>70</v>
       </c>
       <c r="D42">
-        <f>(B5-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>304.85159999999979</v>
       </c>
       <c r="E42" t="s">
@@ -8746,7 +8746,7 @@
         <v>78</v>
       </c>
       <c r="D43">
-        <f>(B6-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>181.17159999999984</v>
       </c>
       <c r="E43" t="s">
@@ -8765,7 +8765,7 @@
         <v>72</v>
       </c>
       <c r="D44">
-        <f>(B7-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>1053.6515999999997</v>
       </c>
     </row>
@@ -8777,7 +8777,7 @@
         <v>77</v>
       </c>
       <c r="D45">
-        <f>(B8-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>1119.5715999999995</v>
       </c>
     </row>
@@ -8789,7 +8789,7 @@
         <v>88</v>
       </c>
       <c r="D46">
-        <f>(B9-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>867.89159999999958</v>
       </c>
     </row>
@@ -8801,7 +8801,7 @@
         <v>82</v>
       </c>
       <c r="D47">
-        <f>(B10-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>927.81159999999966</v>
       </c>
     </row>
@@ -8813,7 +8813,7 @@
         <v>82</v>
       </c>
       <c r="D48">
-        <f>(B11-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>181.17159999999984</v>
       </c>
     </row>
@@ -8825,7 +8825,7 @@
         <v>83</v>
       </c>
       <c r="D49">
-        <f>(B12-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>109.41159999999986</v>
       </c>
     </row>
@@ -8837,7 +8837,7 @@
         <v>111</v>
       </c>
       <c r="D50">
-        <f>(B13-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>648.21159999999963</v>
       </c>
     </row>
@@ -8849,229 +8849,229 @@
         <v>97</v>
       </c>
       <c r="D51">
-        <f>(B14-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>754.05159999999967</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D52">
-        <f>(B15-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>1257.4115999999995</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D53">
-        <f>(B16-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>1187.4915999999996</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D54">
-        <f>(B17-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>700.13159999999971</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D55">
-        <f>(B18-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>109.41159999999986</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D56">
-        <f>(B19-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>270.93159999999978</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D57">
-        <f>(B20-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>504.4515999999997</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D58">
-        <f>(B21-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>89.491599999999877</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D59">
-        <f>(B22-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>504.4515999999997</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D60">
-        <f>(B23-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>30.691600000000069</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D61">
-        <f>(B24-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>6.0515999999999694</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D62">
-        <f>(B25-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>211.41160000000019</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D63">
-        <f>(B26-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>12.531600000000044</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D64">
-        <f>(B27-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>381.81160000000023</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65">
-        <f>(B28-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>508.05160000000029</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66">
-        <f>(B29-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>72.931600000000103</v>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67">
-        <f>(B30-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>273.57160000000022</v>
       </c>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68">
-        <f>(B31-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>343.73160000000024</v>
       </c>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69">
-        <f>(B32-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>111.09160000000013</v>
       </c>
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70">
-        <f>(B33-$E$5)^2</f>
+        <f t="shared" si="9"/>
         <v>1124.9316000000003</v>
       </c>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71">
-        <f>(B34-$E$5)^2</f>
+        <f t="shared" ref="D71:D102" si="10">(B34-$E$5)^2</f>
         <v>994.77160000000038</v>
       </c>
     </row>
     <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72">
-        <f>(B35-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>994.77160000000038</v>
       </c>
     </row>
     <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73">
-        <f>(B36-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>1725.5716000000004</v>
       </c>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74">
-        <f>(B37-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>1563.4116000000006</v>
       </c>
     </row>
     <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75">
-        <f>(B38-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>872.61160000000041</v>
       </c>
     </row>
     <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76">
-        <f>(B39-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>814.53160000000037</v>
       </c>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77">
-        <f>(B40-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>652.29160000000036</v>
       </c>
     </row>
     <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78">
-        <f>(B41-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>343.73160000000024</v>
       </c>
     </row>
     <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79">
-        <f>(B42-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>463.97160000000025</v>
       </c>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80">
-        <f>(B43-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>183.33160000000018</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81">
-        <f>(B44-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>381.81160000000023</v>
       </c>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82">
-        <f>(B45-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>211.41160000000019</v>
       </c>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83">
-        <f>(B46-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>12.531600000000044</v>
       </c>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84">
-        <f>(B47-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>91.011600000000115</v>
       </c>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85">
-        <f>(B48-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>91.011600000000115</v>
       </c>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86">
-        <f>(B49-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>72.931600000000103</v>
       </c>
     </row>
     <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87">
-        <f>(B50-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>378.69159999999977</v>
       </c>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88">
-        <f>(B51-$E$5)^2</f>
+        <f t="shared" si="10"/>
         <v>29.811599999999931</v>
       </c>
     </row>

</xml_diff>